<commit_message>
Appenzeller and Bos Priors without Placeholder Titles
</commit_message>
<xml_diff>
--- a/simulations/cleaned_inclusion_exclusion/Appenzeller-Herzog_2019 IEC_clean/output/tables/metrics/metrics_sim.xlsx
+++ b/simulations/cleaned_inclusion_exclusion/Appenzeller-Herzog_2019 IEC_clean/output/tables/metrics/metrics_sim.xlsx
@@ -621,13 +621,13 @@
         <v>0.7983281086729362</v>
       </c>
       <c r="I2">
-        <v>0.05524947294448349</v>
+        <v>0.05501054111033029</v>
       </c>
       <c r="J2">
         <v>0.8</v>
       </c>
       <c r="K2">
-        <v>170.24</v>
+        <v>169.56</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -713,7 +713,7 @@
         <v>36</v>
       </c>
       <c r="C3">
-        <v>0.9230769230769231</v>
+        <v>0.8846153846153846</v>
       </c>
       <c r="D3">
         <v>0.9615384615384616</v>
@@ -728,16 +728,16 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.8103028193525931</v>
+        <v>0.8016011138183083</v>
       </c>
       <c r="I3">
-        <v>0.06292723784820729</v>
+        <v>0.06219772500067548</v>
       </c>
       <c r="J3">
-        <v>0.8076923076923077</v>
+        <v>0.7692307692307693</v>
       </c>
       <c r="K3">
-        <v>192.6538461538462</v>
+        <v>190.5769230769231</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -755,34 +755,34 @@
         <v>23</v>
       </c>
       <c r="Q3">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="R3">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="S3">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="T3">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="U3">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="V3">
-        <v>2810</v>
+        <v>2815</v>
       </c>
       <c r="W3">
-        <v>2804</v>
+        <v>2807</v>
       </c>
       <c r="X3">
-        <v>2754</v>
+        <v>2757</v>
       </c>
       <c r="Y3">
-        <v>2710</v>
+        <v>2692</v>
       </c>
       <c r="Z3">
-        <v>2612</v>
+        <v>2600</v>
       </c>
       <c r="AA3">
         <v>24</v>
@@ -800,19 +800,19 @@
         <v>3</v>
       </c>
       <c r="AF3">
-        <v>0.987004</v>
+        <v>0.98876</v>
       </c>
       <c r="AG3">
-        <v>0.984896</v>
+        <v>0.98595</v>
       </c>
       <c r="AH3">
-        <v>0.967334</v>
+        <v>0.968388</v>
       </c>
       <c r="AI3">
-        <v>0.951879</v>
+        <v>0.945557</v>
       </c>
       <c r="AJ3">
-        <v>0.917457</v>
+        <v>0.913242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting Relevance Markers Appenzeller-Herzog (2019) - van Dis (2020)
</commit_message>
<xml_diff>
--- a/simulations/cleaned_inclusion_exclusion/Appenzeller-Herzog_2019 IEC_clean/output/tables/metrics/metrics_sim.xlsx
+++ b/simulations/cleaned_inclusion_exclusion/Appenzeller-Herzog_2019 IEC_clean/output/tables/metrics/metrics_sim.xlsx
@@ -728,16 +728,16 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.8016011138183083</v>
+        <v>0.7935955447267664</v>
       </c>
       <c r="I3">
-        <v>0.06219772500067548</v>
+        <v>0.06059009483667018</v>
       </c>
       <c r="J3">
         <v>0.7692307692307693</v>
       </c>
       <c r="K3">
-        <v>190.5769230769231</v>
+        <v>186</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -755,34 +755,34 @@
         <v>23</v>
       </c>
       <c r="Q3">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R3">
         <v>40</v>
       </c>
       <c r="S3">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="T3">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="U3">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="V3">
-        <v>2815</v>
+        <v>2819</v>
       </c>
       <c r="W3">
         <v>2807</v>
       </c>
       <c r="X3">
-        <v>2757</v>
+        <v>2764</v>
       </c>
       <c r="Y3">
-        <v>2692</v>
+        <v>2720</v>
       </c>
       <c r="Z3">
-        <v>2600</v>
+        <v>2608</v>
       </c>
       <c r="AA3">
         <v>24</v>
@@ -800,19 +800,19 @@
         <v>3</v>
       </c>
       <c r="AF3">
-        <v>0.98876</v>
+        <v>0.990165</v>
       </c>
       <c r="AG3">
         <v>0.98595</v>
       </c>
       <c r="AH3">
-        <v>0.968388</v>
+        <v>0.970847</v>
       </c>
       <c r="AI3">
-        <v>0.945557</v>
+        <v>0.955392</v>
       </c>
       <c r="AJ3">
-        <v>0.913242</v>
+        <v>0.916052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>